<commit_message>
Adding ARIC data validation preprocessing
</commit_message>
<xml_diff>
--- a/Data/Preprocessed Data/Data_Dictionary_Ref.xlsx
+++ b/Data/Preprocessed Data/Data_Dictionary_Ref.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/Data/Preprocessed Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3838ABD7-2AE3-B74D-B169-34729A7CA2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772905C9-E0CD-574F-B70F-9D0DF054D21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{3C7A453F-F56A-6346-B453-C1F685D97160}"/>
   </bookViews>
@@ -1040,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32E90D8-0482-BA4B-B75F-C9DD8C8422E0}">
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1048,7 +1048,7 @@
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="3" max="3" width="77" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>